<commit_message>
Updated ITA model - 2025-08-05 00:47
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A150732A-3720-4504-8773-B7D6C7BA865E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38A6B79-64D1-471F-B302-83244C7305B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
   <sheets>
     <sheet name="ev_charging_uc" sheetId="9" r:id="rId1"/>
     <sheet name="customize" sheetId="10" r:id="rId2"/>
+    <sheet name="timeslice_def" sheetId="11" r:id="rId3"/>
+    <sheet name="re_profiles" sheetId="12" r:id="rId4"/>
+    <sheet name="load_shapes" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="151">
   <si>
     <t>UC_N</t>
   </si>
@@ -75,24 +78,6 @@
     <t>day</t>
   </si>
   <si>
-    <t>daynight</t>
-  </si>
-  <si>
-    <t>TimeSlices</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>RaD,SaD,TaD,Tc0916h07,Tc0916h08,Tc0916h09,Tc0916h10,Tc0916h11,Tc0916h12,Tc0916h13,Tc0916h14,Tc0916h15,Tc0916h16,Tc0916h17,Tc0916h18,Tc0917h07,Tc0917h08,Tc0917h09,Tc0917h10,Tc0917h11,Tc0917h12,Tc0917h13,Tc0917h14,Tc0917h15,Tc0917h16,Tc0917h17,Tc0917h18,WaD,Wb0121h07,Wb0121h08,Wb0121h09,Wb0121h10,Wb0121h11,Wb0121h12,Wb0121h13,Wb0121h14,Wb0121h15,Wb0121h16,Wb0121h17,Wb0121h18,Wb0122h07,Wb0122h08,Wb0122h09,Wb0122h10,Wb0122h11,Wb0122h12,Wb0122h13,Wb0122h14,Wb0122h15,Wb0122h16,Wb0122h17,Wb0122h18</t>
-  </si>
-  <si>
-    <t>Night</t>
-  </si>
-  <si>
-    <t>RaD,RaN,RaP,SaD,SaN,SaP,TaD,TaN,TaP,Tc0916h01,Tc0916h02,Tc0916h03,Tc0916h04,Tc0916h05,Tc0916h06,Tc0916h19,Tc0916h20,Tc0916h21,Tc0916h22,Tc0916h23,Tc0916h24,Tc0917h01,Tc0917h02,Tc0917h03,Tc0917h04,Tc0917h05,Tc0917h06,Tc0917h19,Tc0917h20,Tc0917h21,Tc0917h22,Tc0917h23,Tc0917h24,WaD,WaN,WaP,Wb0121h01,Wb0121h02,Wb0121h03,Wb0121h04,Wb0121h05,Wb0121h06,Wb0121h19,Wb0121h20,Wb0121h21,Wb0121h22,Wb0121h23,Wb0121h24,Wb0122h01,Wb0122h02,Wb0122h03,Wb0122h04,Wb0122h05,Wb0122h06,Wb0122h19,Wb0122h20,Wb0122h21,Wb0122h22,Wb0122h23,Wb0122h24</t>
-  </si>
-  <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
   <si>
@@ -268,6 +253,246 @@
   </si>
   <si>
     <t>timeslice</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>wparent</t>
+  </si>
+  <si>
+    <t>dparent</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>S1,S2,S3,S4,S5</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>~TimeSlices</t>
+  </si>
+  <si>
+    <t>com_fr</t>
+  </si>
+  <si>
+    <t>commodity</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>S1aH1</t>
+  </si>
+  <si>
+    <t>elc_sol-ITA</t>
+  </si>
+  <si>
+    <t>IMPNRGZ</t>
+  </si>
+  <si>
+    <t>S1aH2</t>
+  </si>
+  <si>
+    <t>S1aH3</t>
+  </si>
+  <si>
+    <t>S1aH4</t>
+  </si>
+  <si>
+    <t>S1aH5</t>
+  </si>
+  <si>
+    <t>S1aH6</t>
+  </si>
+  <si>
+    <t>S1aH7</t>
+  </si>
+  <si>
+    <t>S1aH8</t>
+  </si>
+  <si>
+    <t>S2aH1</t>
+  </si>
+  <si>
+    <t>S2aH2</t>
+  </si>
+  <si>
+    <t>S2aH3</t>
+  </si>
+  <si>
+    <t>S2aH4</t>
+  </si>
+  <si>
+    <t>S2aH5</t>
+  </si>
+  <si>
+    <t>S2aH6</t>
+  </si>
+  <si>
+    <t>S2aH7</t>
+  </si>
+  <si>
+    <t>S2aH8</t>
+  </si>
+  <si>
+    <t>S3aH1</t>
+  </si>
+  <si>
+    <t>S3aH2</t>
+  </si>
+  <si>
+    <t>S3aH3</t>
+  </si>
+  <si>
+    <t>S3aH4</t>
+  </si>
+  <si>
+    <t>S3aH5</t>
+  </si>
+  <si>
+    <t>S3aH6</t>
+  </si>
+  <si>
+    <t>S3aH7</t>
+  </si>
+  <si>
+    <t>S3aH8</t>
+  </si>
+  <si>
+    <t>S4aH1</t>
+  </si>
+  <si>
+    <t>S4aH2</t>
+  </si>
+  <si>
+    <t>S4aH3</t>
+  </si>
+  <si>
+    <t>S4aH4</t>
+  </si>
+  <si>
+    <t>S4aH5</t>
+  </si>
+  <si>
+    <t>S4aH6</t>
+  </si>
+  <si>
+    <t>S4aH7</t>
+  </si>
+  <si>
+    <t>S4aH8</t>
+  </si>
+  <si>
+    <t>S5aH1</t>
+  </si>
+  <si>
+    <t>S5aH2</t>
+  </si>
+  <si>
+    <t>S5aH3</t>
+  </si>
+  <si>
+    <t>S5aH4</t>
+  </si>
+  <si>
+    <t>S5aH5</t>
+  </si>
+  <si>
+    <t>S5aH6</t>
+  </si>
+  <si>
+    <t>S5aH7</t>
+  </si>
+  <si>
+    <t>S5aH8</t>
+  </si>
+  <si>
+    <t>~TFM_DINS-AT</t>
+  </si>
+  <si>
+    <t>elc_win-ITA</t>
+  </si>
+  <si>
+    <t>g_yrfr</t>
+  </si>
+  <si>
+    <t>elc_roadtransport</t>
+  </si>
+  <si>
+    <t>day_night</t>
+  </si>
+  <si>
+    <t>S1aH4,S2aH2,S3aH2,S3aH3,S1aH2,S2aH3,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S5aH4,S1aH3,S3aH5,S5aH3,S3aH4,S4aH3,S4aH4,S4aH5,S4aH2</t>
+  </si>
+  <si>
+    <t>S4aH8,S1aH1,S2aH7,S4aH1,S3aH8,S4aH6,S1aH6,S1aH7,S3aH6,S4aH7,S5aH6,S5aH7,S1aH8,S5aH1,S2aH8,S2aH6,S3aH1,S2aH1,S3aH7,S5aH8</t>
+  </si>
+  <si>
+    <t>elc_buildings</t>
+  </si>
+  <si>
+    <t>elc_industry</t>
+  </si>
+  <si>
+    <t>com_pkflx</t>
+  </si>
+  <si>
+    <t>ncap_afs</t>
+  </si>
+  <si>
+    <t>pset_ci</t>
+  </si>
+  <si>
+    <t>hydro</t>
+  </si>
+  <si>
+    <t>~TFM_INS-AT</t>
   </si>
 </sst>
 </file>
@@ -744,7 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEB9B52-0D25-4BAC-94A8-E3500D4397D3}">
   <dimension ref="B1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -760,13 +985,13 @@
     </row>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -780,7 +1005,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>2</v>
@@ -795,7 +1020,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.45">
@@ -803,21 +1028,21 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D7" t="str">
         <f>F7</f>
         <v>AuxStoIN</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>RaD,RaN,RaP,SaD,SaN,SaP,TaD,TaN,TaP,Tc0916h01,Tc0916h02,Tc0916h03,Tc0916h04,Tc0916h05,Tc0916h06,Tc0916h19,Tc0916h20,Tc0916h21,Tc0916h22,Tc0916h23,Tc0916h24,Tc0917h01,Tc0917h02,Tc0917h03,Tc0917h04,Tc0917h05,Tc0917h06,Tc0917h19,Tc0917h20,Tc0917h21,Tc0917h22,Tc0917h23,Tc0917h24,WaD,WaN,WaP,Wb0121h01,Wb0121h02,Wb0121h03,Wb0121h04,Wb0121h05,Wb0121h06,Wb0121h19,Wb0121h20,Wb0121h21,Wb0121h22,Wb0121h23,Wb0121h24,Wb0122h01,Wb0122h02,Wb0122h03,Wb0122h04,Wb0122h05,Wb0122h06,Wb0122h19,Wb0122h20,Wb0122h21,Wb0122h22,Wb0122h23,Wb0122h24</v>
+        <v>S4aH8,S1aH1,S2aH7,S4aH1,S3aH8,S4aH6,S1aH6,S1aH7,S3aH6,S4aH7,S5aH6,S5aH7,S1aH8,S5aH1,S2aH8,S2aH6,S3aH1,S2aH1,S3aH7,S5aH8</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -835,21 +1060,21 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D8" t="str">
         <f>F8</f>
         <v>AuxStoIN</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>RaD,SaD,TaD,Tc0916h07,Tc0916h08,Tc0916h09,Tc0916h10,Tc0916h11,Tc0916h12,Tc0916h13,Tc0916h14,Tc0916h15,Tc0916h16,Tc0916h17,Tc0916h18,Tc0917h07,Tc0917h08,Tc0917h09,Tc0917h10,Tc0917h11,Tc0917h12,Tc0917h13,Tc0917h14,Tc0917h15,Tc0917h16,Tc0917h17,Tc0917h18,WaD,Wb0121h07,Wb0121h08,Wb0121h09,Wb0121h10,Wb0121h11,Wb0121h12,Wb0121h13,Wb0121h14,Wb0121h15,Wb0121h16,Wb0121h17,Wb0121h18,Wb0122h07,Wb0122h08,Wb0122h09,Wb0122h10,Wb0122h11,Wb0122h12,Wb0122h13,Wb0122h14,Wb0122h15,Wb0122h16,Wb0122h17,Wb0122h18</v>
+        <v>S1aH4,S2aH2,S3aH2,S3aH3,S1aH2,S2aH3,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S5aH4,S1aH3,S3aH5,S5aH3,S3aH4,S4aH3,S4aH4,S4aH5,S4aH2</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -861,26 +1086,26 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -908,553 +1133,3593 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B52" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF254FA-A496-4720-97CA-89CEBA41A707}">
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="5"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F455B98B-057F-4E65-8770-55D54CCE6FFE}">
+  <dimension ref="B2:O43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4">
+        <v>4.0774999999999999E-2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K4" t="s">
+        <v>97</v>
+      </c>
+      <c r="M4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N4">
+        <v>0.14770939379916706</v>
+      </c>
+      <c r="O4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5">
+        <v>8.8889999999999998E-5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5">
+        <v>5.3729999999999993E-3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>138</v>
+      </c>
+      <c r="K5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" t="s">
+        <v>80</v>
+      </c>
+      <c r="N5">
+        <v>0.45489356779268852</v>
+      </c>
+      <c r="O5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6">
+        <v>2.2627109999999999E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6">
+        <v>1.4475999999999999E-2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>138</v>
+      </c>
+      <c r="K6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M6" t="s">
+        <v>86</v>
+      </c>
+      <c r="N6">
+        <v>7.7845904673762151E-2</v>
+      </c>
+      <c r="O6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>3.1515769999999999E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>2.1163000000000001E-2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>138</v>
+      </c>
+      <c r="K7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M7" t="s">
+        <v>82</v>
+      </c>
+      <c r="N7">
+        <v>0.13802637667746412</v>
+      </c>
+      <c r="O7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8">
+        <v>6.8002030000000005E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8">
+        <v>7.1017999999999998E-2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K8" t="s">
+        <v>97</v>
+      </c>
+      <c r="M8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N8">
+        <v>0.38152475705691813</v>
+      </c>
+      <c r="O8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9">
+        <v>2.6397600000000001E-3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9">
+        <v>1.0756E-2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>138</v>
+      </c>
+      <c r="K9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10">
+        <v>1.1674E-2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>138</v>
+      </c>
+      <c r="K10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11">
+        <v>3.3270000000000001E-2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>138</v>
+      </c>
+      <c r="K11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12">
+        <v>1.378014E-2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12">
+        <v>6.4889000000000002E-2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>138</v>
+      </c>
+      <c r="K12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13">
+        <v>2.2232410000000001E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13">
+        <v>9.8399999999999998E-3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>138</v>
+      </c>
+      <c r="K13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14">
+        <v>6.1518330000000003E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" t="s">
+        <v>107</v>
+      </c>
+      <c r="I14">
+        <v>3.3799000000000003E-2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>138</v>
+      </c>
+      <c r="K14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15">
+        <v>6.7698190000000005E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15">
+        <v>5.2359999999999997E-2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>138</v>
+      </c>
+      <c r="K15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16">
+        <v>0.15982843999999999</v>
+      </c>
+      <c r="D16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" t="s">
+        <v>109</v>
+      </c>
+      <c r="I16">
+        <v>0.17358999999999999</v>
+      </c>
+      <c r="J16" t="s">
+        <v>138</v>
+      </c>
+      <c r="K16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17">
+        <v>2.2495669999999999E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17">
+        <v>2.5507999999999999E-2</v>
+      </c>
+      <c r="J17" t="s">
+        <v>138</v>
+      </c>
+      <c r="K17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18">
+        <v>1.179971E-2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18">
+        <v>2.0265999999999999E-2</v>
+      </c>
+      <c r="J18" t="s">
+        <v>138</v>
+      </c>
+      <c r="K18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19">
+        <v>2.4689500000000001E-3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19">
+        <v>4.6764E-2</v>
+      </c>
+      <c r="J19" t="s">
+        <v>138</v>
+      </c>
+      <c r="K19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20">
+        <v>6.9502299999999999E-3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20">
+        <v>1.0950000000000001E-3</v>
+      </c>
+      <c r="J20" t="s">
+        <v>138</v>
+      </c>
+      <c r="K20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21">
+        <v>8.8978100000000008E-3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21">
+        <v>1.4E-5</v>
+      </c>
+      <c r="J21" t="s">
+        <v>138</v>
+      </c>
+      <c r="K21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22">
+        <v>2.1362920000000001E-2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22">
+        <v>1.08E-4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>138</v>
+      </c>
+      <c r="K22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23">
+        <v>2.2302309999999999E-2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23">
+        <v>8.3600000000000005E-4</v>
+      </c>
+      <c r="J23" t="s">
+        <v>138</v>
+      </c>
+      <c r="K23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24">
+        <v>5.0535759999999999E-2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24">
+        <v>1.8824E-2</v>
+      </c>
+      <c r="J24" t="s">
+        <v>138</v>
+      </c>
+      <c r="K24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25">
+        <v>7.6808800000000002E-3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I25">
+        <v>3.3969999999999998E-3</v>
+      </c>
+      <c r="J25" t="s">
+        <v>138</v>
+      </c>
+      <c r="K25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26">
+        <v>5.4394600000000001E-3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" t="s">
+        <v>119</v>
+      </c>
+      <c r="I26">
+        <v>1.915E-3</v>
+      </c>
+      <c r="J26" t="s">
+        <v>138</v>
+      </c>
+      <c r="K26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27">
+        <v>1.8646700000000001E-3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" t="s">
+        <v>120</v>
+      </c>
+      <c r="I27">
+        <v>1.9039999999999999E-3</v>
+      </c>
+      <c r="J27" t="s">
+        <v>138</v>
+      </c>
+      <c r="K27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28">
+        <v>5.3654999999999996E-3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" t="s">
+        <v>97</v>
+      </c>
+      <c r="H28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I28">
+        <v>4.8161000000000002E-2</v>
+      </c>
+      <c r="J28" t="s">
+        <v>138</v>
+      </c>
+      <c r="K28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29">
+        <v>1.8131049999999999E-2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
+        <v>97</v>
+      </c>
+      <c r="H29" t="s">
+        <v>122</v>
+      </c>
+      <c r="I29">
+        <v>5.5269999999999998E-3</v>
+      </c>
+      <c r="J29" t="s">
+        <v>138</v>
+      </c>
+      <c r="K29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30">
+        <v>5.9624789999999997E-2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" t="s">
+        <v>123</v>
+      </c>
+      <c r="I30">
+        <v>1.5792E-2</v>
+      </c>
+      <c r="J30" t="s">
+        <v>138</v>
+      </c>
+      <c r="K30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31">
+        <v>6.9100110000000006E-2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" t="s">
+        <v>97</v>
+      </c>
+      <c r="H31" t="s">
+        <v>124</v>
+      </c>
+      <c r="I31">
+        <v>2.8983999999999999E-2</v>
+      </c>
+      <c r="J31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32">
+        <v>0.15711573000000001</v>
+      </c>
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" t="s">
+        <v>97</v>
+      </c>
+      <c r="H32" t="s">
+        <v>125</v>
+      </c>
+      <c r="I32">
+        <v>9.9659999999999999E-2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>138</v>
+      </c>
+      <c r="K32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33">
+        <v>1.427003E-2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" t="s">
+        <v>97</v>
+      </c>
+      <c r="H33" t="s">
+        <v>126</v>
+      </c>
+      <c r="I33">
+        <v>1.4661E-2</v>
+      </c>
+      <c r="J33" t="s">
+        <v>138</v>
+      </c>
+      <c r="K33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34">
+        <v>5.76283E-3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" t="s">
+        <v>127</v>
+      </c>
+      <c r="I34">
+        <v>1.1509999999999999E-2</v>
+      </c>
+      <c r="J34" t="s">
+        <v>138</v>
+      </c>
+      <c r="K34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35">
+        <v>8.2800000000000003E-6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" t="s">
+        <v>97</v>
+      </c>
+      <c r="H35" t="s">
+        <v>128</v>
+      </c>
+      <c r="I35">
+        <v>3.4647999999999998E-2</v>
+      </c>
+      <c r="J35" t="s">
+        <v>138</v>
+      </c>
+      <c r="K35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" t="s">
+        <v>129</v>
+      </c>
+      <c r="I36">
+        <v>2.1659999999999999E-2</v>
+      </c>
+      <c r="J36" t="s">
+        <v>138</v>
+      </c>
+      <c r="K36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" t="s">
+        <v>130</v>
+      </c>
+      <c r="I37">
+        <v>2.5929999999999998E-3</v>
+      </c>
+      <c r="J37" t="s">
+        <v>138</v>
+      </c>
+      <c r="K37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38">
+        <v>1.024945E-2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" t="s">
+        <v>97</v>
+      </c>
+      <c r="H38" t="s">
+        <v>131</v>
+      </c>
+      <c r="I38">
+        <v>5.4539999999999996E-3</v>
+      </c>
+      <c r="J38" t="s">
+        <v>138</v>
+      </c>
+      <c r="K38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39">
+        <v>1.5962420000000001E-2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" t="s">
+        <v>97</v>
+      </c>
+      <c r="H39" t="s">
+        <v>132</v>
+      </c>
+      <c r="I39">
+        <v>5.7080000000000004E-3</v>
+      </c>
+      <c r="J39" t="s">
+        <v>138</v>
+      </c>
+      <c r="K39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40">
+        <v>3.2680319999999999E-2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" t="s">
+        <v>133</v>
+      </c>
+      <c r="I40">
+        <v>2.0205000000000001E-2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>138</v>
+      </c>
+      <c r="K40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" t="s">
+        <v>97</v>
+      </c>
+      <c r="H41" t="s">
+        <v>134</v>
+      </c>
+      <c r="I41">
+        <v>2.849E-3</v>
+      </c>
+      <c r="J41" t="s">
+        <v>138</v>
+      </c>
+      <c r="K41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="H42" t="s">
+        <v>135</v>
+      </c>
+      <c r="I42">
+        <v>2.9480000000000001E-3</v>
+      </c>
+      <c r="J42" t="s">
+        <v>138</v>
+      </c>
+      <c r="K42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" t="s">
+        <v>97</v>
+      </c>
+      <c r="H43" t="s">
+        <v>136</v>
+      </c>
+      <c r="I43">
+        <v>1.3637999999999999E-2</v>
+      </c>
+      <c r="J43" t="s">
+        <v>138</v>
+      </c>
+      <c r="K43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE25A5A5-1BB1-49E6-89D1-5CF19766AECA}">
+  <dimension ref="B2:O83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>5.3881278538812784E-2</v>
+      </c>
+      <c r="C4">
+        <v>2.9864505382492607E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4">
+        <v>4.9413150019647384E-2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O4">
+        <v>0.30170207507267222</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>6.735159817351598E-3</v>
+      </c>
+      <c r="C5">
+        <v>8.6053584599192871E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" t="s">
+        <v>144</v>
+      </c>
+      <c r="I5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5">
+        <v>8.3943858858496045E-3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O5">
+        <v>4.7484009459135335E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>1.3470319634703196E-2</v>
+      </c>
+      <c r="C6">
+        <v>1.6839121895432966E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6">
+        <v>1.700531767651765E-2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>99</v>
+      </c>
+      <c r="O6">
+        <v>4.824655587311355E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>1.3470319634703196E-2</v>
+      </c>
+      <c r="C7">
+        <v>1.6702218465388795E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7">
+        <v>1.6777383906641918E-2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O7">
+        <v>6.0317454394499759E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>3.3675799086757989E-2</v>
+      </c>
+      <c r="C8">
+        <v>5.4037739601720411E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8">
+        <v>4.2415004863410904E-2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" t="s">
+        <v>101</v>
+      </c>
+      <c r="O8">
+        <v>7.7866629521058162E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>6.735159817351598E-3</v>
+      </c>
+      <c r="C9">
+        <v>1.016996908899552E-2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" t="s">
+        <v>140</v>
+      </c>
+      <c r="H9" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J9">
+        <v>8.8413511413772579E-3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O9">
+        <v>4.0331772644039976E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>6.735159817351598E-3</v>
+      </c>
+      <c r="C10">
+        <v>9.1920874458228732E-3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" t="s">
+        <v>144</v>
+      </c>
+      <c r="I10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10">
+        <v>8.5385270462681635E-3</v>
+      </c>
+      <c r="M10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" t="s">
+        <v>103</v>
+      </c>
+      <c r="O10">
+        <v>3.0789916534887052E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <v>2.6940639269406392E-2</v>
+      </c>
+      <c r="C11">
+        <v>1.623283527666592E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11">
+        <v>2.8553373673719802E-2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" t="s">
+        <v>104</v>
+      </c>
+      <c r="O11">
+        <v>0.109785485062313</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <v>0.11141552511415526</v>
+      </c>
+      <c r="C12">
+        <v>6.1753722994306731E-2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J12">
+        <v>9.0904601496028622E-2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" t="s">
+        <v>105</v>
+      </c>
+      <c r="O12">
+        <v>0.39609048684121051</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <v>1.3926940639269407E-2</v>
+      </c>
+      <c r="C13">
+        <v>1.7794131052714456E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13">
+        <v>1.4801270832185959E-2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" t="s">
+        <v>106</v>
+      </c>
+      <c r="O13">
+        <v>0.17260864196062009</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>2.7853881278538814E-2</v>
+      </c>
+      <c r="C14">
+        <v>3.4819879173607154E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I14" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14">
+        <v>2.9861072108283881E-2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" t="s">
+        <v>107</v>
+      </c>
+      <c r="O14">
+        <v>0.16771535784982539</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <v>2.7853881278538814E-2</v>
+      </c>
+      <c r="C15">
+        <v>3.4536790725041226E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" t="s">
+        <v>108</v>
+      </c>
+      <c r="J15">
+        <v>2.9646906653991761E-2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" t="s">
+        <v>108</v>
+      </c>
+      <c r="O15">
+        <v>0.1682397095214816</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B16">
+        <v>6.9634703196347028E-2</v>
+      </c>
+      <c r="C16">
+        <v>0.11173905476965917</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" t="s">
+        <v>144</v>
+      </c>
+      <c r="I16" t="s">
+        <v>109</v>
+      </c>
+      <c r="J16">
+        <v>7.3928865615248154E-2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" t="s">
+        <v>109</v>
+      </c>
+      <c r="O16">
+        <v>0.19323961229369258</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <v>1.3926940639269407E-2</v>
+      </c>
+      <c r="C17">
+        <v>2.1029427607753434E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" t="s">
+        <v>140</v>
+      </c>
+      <c r="H17" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" t="s">
+        <v>110</v>
+      </c>
+      <c r="J17">
+        <v>1.5030507466939664E-2</v>
+      </c>
+      <c r="M17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" t="s">
+        <v>110</v>
+      </c>
+      <c r="O17">
+        <v>0.18025049028347295</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <v>1.3926940639269407E-2</v>
+      </c>
+      <c r="C18">
+        <v>1.9007367260854072E-2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I18" t="s">
+        <v>111</v>
+      </c>
+      <c r="J18">
+        <v>1.4913767770150556E-2</v>
+      </c>
+      <c r="M18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" t="s">
+        <v>111</v>
+      </c>
+      <c r="O18">
+        <v>0.15800839499366748</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B19">
+        <v>5.5707762557077628E-2</v>
+      </c>
+      <c r="C19">
+        <v>3.3566201758529535E-2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" t="s">
+        <v>144</v>
+      </c>
+      <c r="I19" t="s">
+        <v>112</v>
+      </c>
+      <c r="J19">
+        <v>5.1929529158049881E-2</v>
+      </c>
+      <c r="M19" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" t="s">
+        <v>112</v>
+      </c>
+      <c r="O19">
+        <v>0.19990108030983977</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B20">
+        <v>2.8310502283105023E-2</v>
+      </c>
+      <c r="C20">
+        <v>1.5691519777241876E-2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" t="s">
+        <v>140</v>
+      </c>
+      <c r="H20" t="s">
+        <v>144</v>
+      </c>
+      <c r="I20" t="s">
+        <v>113</v>
+      </c>
+      <c r="J20">
+        <v>2.3847087699625354E-2</v>
+      </c>
+      <c r="M20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" t="s">
+        <v>113</v>
+      </c>
+      <c r="O20">
+        <v>0.29079453954855983</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B21">
+        <v>3.5388127853881279E-3</v>
+      </c>
+      <c r="C21">
+        <v>4.521459529788099E-3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" t="s">
+        <v>140</v>
+      </c>
+      <c r="H21" t="s">
+        <v>144</v>
+      </c>
+      <c r="I21" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21">
+        <v>3.9226118087310096E-3</v>
+      </c>
+      <c r="M21" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" t="s">
+        <v>114</v>
+      </c>
+      <c r="O21">
+        <v>7.4383366010698726E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B22">
+        <v>7.0776255707762558E-3</v>
+      </c>
+      <c r="C22">
+        <v>8.8476742162444406E-3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
+        <v>140</v>
+      </c>
+      <c r="H22" t="s">
+        <v>144</v>
+      </c>
+      <c r="I22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22">
+        <v>8.0528034089415845E-3</v>
+      </c>
+      <c r="M22" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" t="s">
+        <v>115</v>
+      </c>
+      <c r="O22">
+        <v>6.822201466584521E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B23">
+        <v>7.0776255707762558E-3</v>
+      </c>
+      <c r="C23">
+        <v>8.775741905543262E-3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" t="s">
+        <v>140</v>
+      </c>
+      <c r="H23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I23" t="s">
+        <v>116</v>
+      </c>
+      <c r="J23">
+        <v>8.1706582379173116E-3</v>
+      </c>
+      <c r="M23" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" t="s">
+        <v>116</v>
+      </c>
+      <c r="O23">
+        <v>7.2534412655806291E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B24">
+        <v>1.7694063926940638E-2</v>
+      </c>
+      <c r="C24">
+        <v>2.8392710638192088E-2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24" t="s">
+        <v>144</v>
+      </c>
+      <c r="I24" t="s">
+        <v>117</v>
+      </c>
+      <c r="J24">
+        <v>2.0148281192040179E-2</v>
+      </c>
+      <c r="M24" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" t="s">
+        <v>117</v>
+      </c>
+      <c r="O24">
+        <v>8.0585218842956552E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B25">
+        <v>3.5388127853881279E-3</v>
+      </c>
+      <c r="C25">
+        <v>5.3435430806586613E-3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" t="s">
+        <v>140</v>
+      </c>
+      <c r="H25" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" t="s">
+        <v>118</v>
+      </c>
+      <c r="J25">
+        <v>3.969488661761114E-3</v>
+      </c>
+      <c r="M25" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" t="s">
+        <v>118</v>
+      </c>
+      <c r="O25">
+        <v>6.0510923392422367E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B26">
+        <v>3.5388127853881279E-3</v>
+      </c>
+      <c r="C26">
+        <v>4.8297408613645603E-3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" t="s">
+        <v>144</v>
+      </c>
+      <c r="I26" t="s">
+        <v>119</v>
+      </c>
+      <c r="J26">
+        <v>3.9291786982744333E-3</v>
+      </c>
+      <c r="M26" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" t="s">
+        <v>119</v>
+      </c>
+      <c r="O26">
+        <v>6.5424670864874468E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <v>1.4155251141552512E-2</v>
+      </c>
+      <c r="C27">
+        <v>8.5291168402820937E-3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" t="s">
+        <v>120</v>
+      </c>
+      <c r="J27">
+        <v>1.4304428038648183E-2</v>
+      </c>
+      <c r="M27" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" t="s">
+        <v>120</v>
+      </c>
+      <c r="O27">
+        <v>0.16837934519996667</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B28">
+        <v>0.11141552511415526</v>
+      </c>
+      <c r="C28">
+        <v>6.1753722994306731E-2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" t="s">
+        <v>144</v>
+      </c>
+      <c r="I28" t="s">
+        <v>121</v>
+      </c>
+      <c r="J28">
+        <v>9.0201913914656887E-2</v>
+      </c>
+      <c r="M28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" t="s">
+        <v>121</v>
+      </c>
+      <c r="O28">
+        <v>0.3257378459195408</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>1.3926940639269407E-2</v>
+      </c>
+      <c r="C29">
+        <v>1.7794131052714456E-2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" t="s">
+        <v>140</v>
+      </c>
+      <c r="H29" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" t="s">
+        <v>122</v>
+      </c>
+      <c r="J29">
+        <v>1.458652054518594E-2</v>
+      </c>
+      <c r="M29" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" t="s">
+        <v>122</v>
+      </c>
+      <c r="O29">
+        <v>0.13113733252573989</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>2.7853881278538814E-2</v>
+      </c>
+      <c r="C30">
+        <v>3.4819879173607154E-2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" t="s">
+        <v>140</v>
+      </c>
+      <c r="H30" t="s">
+        <v>144</v>
+      </c>
+      <c r="I30" t="s">
+        <v>123</v>
+      </c>
+      <c r="J30">
+        <v>2.9773057299849567E-2</v>
+      </c>
+      <c r="M30" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30" t="s">
+        <v>123</v>
+      </c>
+      <c r="O30">
+        <v>0.13375718145694071</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <v>2.7853881278538814E-2</v>
+      </c>
+      <c r="C31">
+        <v>3.4536790725041226E-2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" t="s">
+        <v>144</v>
+      </c>
+      <c r="I31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J31">
+        <v>2.9841001515502973E-2</v>
+      </c>
+      <c r="M31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N31" t="s">
+        <v>124</v>
+      </c>
+      <c r="O31">
+        <v>0.12830972920522465</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>6.9634703196347028E-2</v>
+      </c>
+      <c r="C32">
+        <v>0.11173905476965917</v>
+      </c>
+      <c r="D32" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" t="s">
+        <v>140</v>
+      </c>
+      <c r="H32" t="s">
+        <v>144</v>
+      </c>
+      <c r="I32" t="s">
+        <v>125</v>
+      </c>
+      <c r="J32">
+        <v>7.4324036133024088E-2</v>
+      </c>
+      <c r="M32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N32" t="s">
+        <v>125</v>
+      </c>
+      <c r="O32">
+        <v>0.16794411000882747</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B33">
+        <v>1.3926940639269407E-2</v>
+      </c>
+      <c r="C33">
+        <v>2.1029427607753434E-2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" t="s">
+        <v>140</v>
+      </c>
+      <c r="H33" t="s">
+        <v>144</v>
+      </c>
+      <c r="I33" t="s">
+        <v>126</v>
+      </c>
+      <c r="J33">
+        <v>1.494214258241032E-2</v>
+      </c>
+      <c r="M33" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33" t="s">
+        <v>126</v>
+      </c>
+      <c r="O33">
+        <v>0.16530699032086882</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <v>1.3926940639269407E-2</v>
+      </c>
+      <c r="C34">
+        <v>1.9007367260854072E-2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" t="s">
+        <v>140</v>
+      </c>
+      <c r="H34" t="s">
+        <v>144</v>
+      </c>
+      <c r="I34" t="s">
+        <v>127</v>
+      </c>
+      <c r="J34">
+        <v>1.4815325394749541E-2</v>
+      </c>
+      <c r="M34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N34" t="s">
+        <v>127</v>
+      </c>
+      <c r="O34">
+        <v>0.12381007042058645</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B35">
+        <v>5.5707762557077628E-2</v>
+      </c>
+      <c r="C35">
+        <v>3.3566201758529535E-2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" t="s">
+        <v>140</v>
+      </c>
+      <c r="H35" t="s">
+        <v>144</v>
+      </c>
+      <c r="I35" t="s">
+        <v>128</v>
+      </c>
+      <c r="J35">
+        <v>5.2827105256473848E-2</v>
+      </c>
+      <c r="M35" t="s">
+        <v>14</v>
+      </c>
+      <c r="N35" t="s">
+        <v>128</v>
+      </c>
+      <c r="O35">
+        <v>0.18969821164223233</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B36">
+        <v>2.8310502283105023E-2</v>
+      </c>
+      <c r="C36">
+        <v>1.5691519777241876E-2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" t="s">
+        <v>140</v>
+      </c>
+      <c r="H36" t="s">
+        <v>144</v>
+      </c>
+      <c r="I36" t="s">
+        <v>129</v>
+      </c>
+      <c r="J36">
+        <v>2.5278796395052556E-2</v>
+      </c>
+      <c r="M36" t="s">
+        <v>14</v>
+      </c>
+      <c r="N36" t="s">
+        <v>129</v>
+      </c>
+      <c r="O36">
+        <v>0.3018567715645406</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B37">
+        <v>3.5388127853881279E-3</v>
+      </c>
+      <c r="C37">
+        <v>4.521459529788099E-3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" t="s">
+        <v>140</v>
+      </c>
+      <c r="H37" t="s">
+        <v>144</v>
+      </c>
+      <c r="I37" t="s">
+        <v>130</v>
+      </c>
+      <c r="J37">
+        <v>4.2866483841047468E-3</v>
+      </c>
+      <c r="M37" t="s">
+        <v>14</v>
+      </c>
+      <c r="N37" t="s">
+        <v>130</v>
+      </c>
+      <c r="O37">
+        <v>5.8368729564079569E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B38">
+        <v>7.0776255707762558E-3</v>
+      </c>
+      <c r="C38">
+        <v>8.8476742162444406E-3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>131</v>
+      </c>
+      <c r="E38" t="s">
+        <v>140</v>
+      </c>
+      <c r="H38" t="s">
+        <v>144</v>
+      </c>
+      <c r="I38" t="s">
+        <v>131</v>
+      </c>
+      <c r="J38">
+        <v>8.6358981114670781E-3</v>
+      </c>
+      <c r="M38" t="s">
+        <v>14</v>
+      </c>
+      <c r="N38" t="s">
+        <v>131</v>
+      </c>
+      <c r="O38">
+        <v>6.3279503760392153E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B39">
+        <v>7.0776255707762558E-3</v>
+      </c>
+      <c r="C39">
+        <v>8.775741905543262E-3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" t="s">
+        <v>140</v>
+      </c>
+      <c r="H39" t="s">
+        <v>144</v>
+      </c>
+      <c r="I39" t="s">
+        <v>132</v>
+      </c>
+      <c r="J39">
+        <v>8.4215374151759489E-3</v>
+      </c>
+      <c r="M39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N39" t="s">
+        <v>132</v>
+      </c>
+      <c r="O39">
+        <v>6.5636106328051946E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B40">
+        <v>1.7694063926940638E-2</v>
+      </c>
+      <c r="C40">
+        <v>2.8392710638192088E-2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" t="s">
+        <v>140</v>
+      </c>
+      <c r="H40" t="s">
+        <v>144</v>
+      </c>
+      <c r="I40" t="s">
+        <v>133</v>
+      </c>
+      <c r="J40">
+        <v>2.1316051665275386E-2</v>
+      </c>
+      <c r="M40" t="s">
+        <v>14</v>
+      </c>
+      <c r="N40" t="s">
+        <v>133</v>
+      </c>
+      <c r="O40">
+        <v>8.7961716292424663E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B41">
+        <v>3.5388127853881279E-3</v>
+      </c>
+      <c r="C41">
+        <v>5.3435430806586613E-3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>134</v>
+      </c>
+      <c r="E41" t="s">
+        <v>140</v>
+      </c>
+      <c r="H41" t="s">
+        <v>144</v>
+      </c>
+      <c r="I41" t="s">
+        <v>134</v>
+      </c>
+      <c r="J41">
+        <v>4.5114770552655533E-3</v>
+      </c>
+      <c r="M41" t="s">
+        <v>14</v>
+      </c>
+      <c r="N41" t="s">
+        <v>134</v>
+      </c>
+      <c r="O41">
+        <v>4.44627304048415E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B42">
+        <v>3.5388127853881279E-3</v>
+      </c>
+      <c r="C42">
+        <v>4.8297408613645603E-3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" t="s">
+        <v>140</v>
+      </c>
+      <c r="H42" t="s">
+        <v>144</v>
+      </c>
+      <c r="I42" t="s">
+        <v>135</v>
+      </c>
+      <c r="J42">
+        <v>4.3715673897100236E-3</v>
+      </c>
+      <c r="M42" t="s">
+        <v>14</v>
+      </c>
+      <c r="N42" t="s">
+        <v>135</v>
+      </c>
+      <c r="O42">
+        <v>3.5079218054054673E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B43">
+        <v>1.4155251141552512E-2</v>
+      </c>
+      <c r="C43">
+        <v>8.5291168402820937E-3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>136</v>
+      </c>
+      <c r="E43" t="s">
+        <v>140</v>
+      </c>
+      <c r="H43" t="s">
+        <v>144</v>
+      </c>
+      <c r="I43" t="s">
+        <v>136</v>
+      </c>
+      <c r="J43">
+        <v>1.4567367881845251E-2</v>
+      </c>
+      <c r="M43" t="s">
+        <v>14</v>
+      </c>
+      <c r="N43" t="s">
+        <v>136</v>
+      </c>
+      <c r="O43">
+        <v>0.11194355190956351</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="H44" t="s">
+        <v>145</v>
+      </c>
+      <c r="I44" t="s">
+        <v>95</v>
+      </c>
+      <c r="J44">
+        <v>5.3084237148893397E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="H45" t="s">
+        <v>145</v>
+      </c>
+      <c r="I45" t="s">
+        <v>98</v>
+      </c>
+      <c r="J45">
+        <v>6.8128512704278962E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="H46" t="s">
+        <v>145</v>
+      </c>
+      <c r="I46" t="s">
+        <v>99</v>
+      </c>
+      <c r="J46">
+        <v>1.3643016669286061E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="H47" t="s">
+        <v>145</v>
+      </c>
+      <c r="I47" t="s">
+        <v>100</v>
+      </c>
+      <c r="J47">
+        <v>1.3624792013555292E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="H48" t="s">
+        <v>145</v>
+      </c>
+      <c r="I48" t="s">
+        <v>101</v>
+      </c>
+      <c r="J48">
+        <v>3.4099682858947933E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H49" t="s">
+        <v>145</v>
+      </c>
+      <c r="I49" t="s">
+        <v>102</v>
+      </c>
+      <c r="J49">
+        <v>6.8485887915071438E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H50" t="s">
+        <v>145</v>
+      </c>
+      <c r="I50" t="s">
+        <v>103</v>
+      </c>
+      <c r="J50">
+        <v>6.8243762104431196E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H51" t="s">
+        <v>145</v>
+      </c>
+      <c r="I51" t="s">
+        <v>104</v>
+      </c>
+      <c r="J51">
+        <v>2.6849692925335147E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H52" t="s">
+        <v>145</v>
+      </c>
+      <c r="I52" t="s">
+        <v>105</v>
+      </c>
+      <c r="J52">
+        <v>0.11009359446781739</v>
+      </c>
+    </row>
+    <row r="53" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H53" t="s">
+        <v>145</v>
+      </c>
+      <c r="I53" t="s">
+        <v>106</v>
+      </c>
+      <c r="J53">
+        <v>1.4036603426470031E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H54" t="s">
+        <v>145</v>
+      </c>
+      <c r="I54" t="s">
+        <v>107</v>
+      </c>
+      <c r="J54">
+        <v>2.8093877894088494E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H55" t="s">
+        <v>145</v>
+      </c>
+      <c r="I55" t="s">
+        <v>108</v>
+      </c>
+      <c r="J55">
+        <v>2.8076754096785336E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H56" t="s">
+        <v>145</v>
+      </c>
+      <c r="I56" t="s">
+        <v>109</v>
+      </c>
+      <c r="J56">
+        <v>7.0176821463893937E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H57" t="s">
+        <v>145</v>
+      </c>
+      <c r="I57" t="s">
+        <v>110</v>
+      </c>
+      <c r="J57">
+        <v>1.4054932253969107E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H58" t="s">
+        <v>145</v>
+      </c>
+      <c r="I58" t="s">
+        <v>111</v>
+      </c>
+      <c r="J58">
+        <v>1.4045598223363393E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H59" t="s">
+        <v>145</v>
+      </c>
+      <c r="I59" t="s">
+        <v>112</v>
+      </c>
+      <c r="J59">
+        <v>5.5564690032008805E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H60" t="s">
+        <v>145</v>
+      </c>
+      <c r="I60" t="s">
+        <v>113</v>
+      </c>
+      <c r="J60">
+        <v>2.7919657774016834E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H61" t="s">
+        <v>145</v>
+      </c>
+      <c r="I61" t="s">
+        <v>114</v>
+      </c>
+      <c r="J61">
+        <v>3.5652537842164418E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H62" t="s">
+        <v>145</v>
+      </c>
+      <c r="I62" t="s">
+        <v>115</v>
+      </c>
+      <c r="J62">
+        <v>7.1471048029648366E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H63" t="s">
+        <v>145</v>
+      </c>
+      <c r="I63" t="s">
+        <v>116</v>
+      </c>
+      <c r="J63">
+        <v>7.1565279949976019E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H64" t="s">
+        <v>145</v>
+      </c>
+      <c r="I64" t="s">
+        <v>117</v>
+      </c>
+      <c r="J64">
+        <v>1.7869063103792035E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H65" t="s">
+        <v>145</v>
+      </c>
+      <c r="I65" t="s">
+        <v>118</v>
+      </c>
+      <c r="J65">
+        <v>3.5690018664276965E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H66" t="s">
+        <v>145</v>
+      </c>
+      <c r="I66" t="s">
+        <v>119</v>
+      </c>
+      <c r="J66">
+        <v>3.5657788459535246E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H67" t="s">
+        <v>145</v>
+      </c>
+      <c r="I67" t="s">
+        <v>120</v>
+      </c>
+      <c r="J67">
+        <v>1.4150194688004086E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H68" t="s">
+        <v>145</v>
+      </c>
+      <c r="I68" t="s">
+        <v>121</v>
+      </c>
+      <c r="J68">
+        <v>0.11003032894153919</v>
+      </c>
+    </row>
+    <row r="69" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H69" t="s">
+        <v>145</v>
+      </c>
+      <c r="I69" t="s">
+        <v>122</v>
+      </c>
+      <c r="J69">
+        <v>1.4018547682109401E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H70" t="s">
+        <v>145</v>
+      </c>
+      <c r="I70" t="s">
+        <v>123</v>
+      </c>
+      <c r="J70">
+        <v>2.8085070216109214E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H71" t="s">
+        <v>145</v>
+      </c>
+      <c r="I71" t="s">
+        <v>124</v>
+      </c>
+      <c r="J71">
+        <v>2.8090502758816051E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H72" t="s">
+        <v>145</v>
+      </c>
+      <c r="I72" t="s">
+        <v>125</v>
+      </c>
+      <c r="J72">
+        <v>7.0203991757650464E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H73" t="s">
+        <v>145</v>
+      </c>
+      <c r="I73" t="s">
+        <v>126</v>
+      </c>
+      <c r="J73">
+        <v>1.4046981771547846E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H74" t="s">
+        <v>145</v>
+      </c>
+      <c r="I74" t="s">
+        <v>127</v>
+      </c>
+      <c r="J74">
+        <v>1.4036841985823589E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H75" t="s">
+        <v>145</v>
+      </c>
+      <c r="I75" t="s">
+        <v>128</v>
+      </c>
+      <c r="J75">
+        <v>5.5632915815616614E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H76" t="s">
+        <v>145</v>
+      </c>
+      <c r="I76" t="s">
+        <v>129</v>
+      </c>
+      <c r="J76">
+        <v>2.7912858509718089E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H77" t="s">
+        <v>145</v>
+      </c>
+      <c r="I77" t="s">
+        <v>130</v>
+      </c>
+      <c r="J77">
+        <v>3.5792015584238993E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H78" t="s">
+        <v>145</v>
+      </c>
+      <c r="I78" t="s">
+        <v>131</v>
+      </c>
+      <c r="J78">
+        <v>7.1634084652425324E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H79" t="s">
+        <v>145</v>
+      </c>
+      <c r="I79" t="s">
+        <v>132</v>
+      </c>
+      <c r="J79">
+        <v>7.1462690571844666E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H80" t="s">
+        <v>145</v>
+      </c>
+      <c r="I80" t="s">
+        <v>133</v>
+      </c>
+      <c r="J80">
+        <v>1.7886637736694772E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H81" t="s">
+        <v>145</v>
+      </c>
+      <c r="I81" t="s">
+        <v>134</v>
+      </c>
+      <c r="J81">
+        <v>3.5971779431103182E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H82" t="s">
+        <v>145</v>
+      </c>
+      <c r="I82" t="s">
+        <v>135</v>
+      </c>
+      <c r="J82">
+        <v>3.5859913361869712E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H83" t="s">
+        <v>145</v>
+      </c>
+      <c r="I83" t="s">
+        <v>136</v>
+      </c>
+      <c r="J83">
+        <v>1.411058185706111E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-05 11:23
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE8DDA9-8ED8-4D54-9E4E-FF2444470079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69C5867-29D3-4C43-B833-6F3F3C1AE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1b0318h14,S3aH2,S4c0909h12,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S3aH3,S4c0909h16,S1aH2,S2aH3,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4c0909h08,S6d1115h08,S4aH2,S6d1115h07,S6d1115h15,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1aH3,S4c0909h14,S6d1115h09,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S1b0318h10,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S6d1115h11</t>
-  </si>
-  <si>
-    <t>S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1b0318h04,S4aH8,S4c0909h05,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S2aH1,S3aH7,S4c0909h21,S5aH8,S1aH6,S4c0909h02,S6d1115h06,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S6d1115h02,S6d1115h22,S6d1115h23,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S6aH8,S1b0318h21,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20</t>
+    <t>S4aH2,S6d1115h07,S6d1115h15,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S4c0909h08,S6d1115h08,S1aH3,S4c0909h14,S6d1115h09,S1aH2,S2aH3,S1b0318h10,S3aH3,S4c0909h16,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1b0318h14,S3aH2,S4c0909h12,S6d1115h11,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18</t>
+  </si>
+  <si>
+    <t>S2aH1,S3aH7,S4c0909h21,S5aH8,S1b0318h04,S4aH8,S4c0909h05,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S6d1115h02,S6d1115h22,S6d1115h23,S6d1115h06,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S6aH8,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S1b0318h21,S1aH6,S4c0909h02,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1b0318h04,S4aH8,S4c0909h05,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S2aH1,S3aH7,S4c0909h21,S5aH8,S1aH6,S4c0909h02,S6d1115h06,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S6d1115h02,S6d1115h22,S6d1115h23,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S6aH8,S1b0318h21,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20</v>
+        <v>S2aH1,S3aH7,S4c0909h21,S5aH8,S1b0318h04,S4aH8,S4c0909h05,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S6d1115h02,S6d1115h22,S6d1115h23,S6d1115h06,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S6aH8,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S1b0318h21,S1aH6,S4c0909h02,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1b0318h14,S3aH2,S4c0909h12,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S3aH3,S4c0909h16,S1aH2,S2aH3,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4c0909h08,S6d1115h08,S4aH2,S6d1115h07,S6d1115h15,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1aH3,S4c0909h14,S6d1115h09,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S1b0318h10,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S6d1115h11</v>
+        <v>S4aH2,S6d1115h07,S6d1115h15,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S4c0909h08,S6d1115h08,S1aH3,S4c0909h14,S6d1115h09,S1aH2,S2aH3,S1b0318h10,S3aH3,S4c0909h16,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1b0318h14,S3aH2,S4c0909h12,S6d1115h11,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F981A35A-1251-43D5-9F6D-8E9572CCE45A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E83548-7D24-4153-9F00-316021126006}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21AC614-4EFC-44AF-8567-0A949759115E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912B446D-27B7-4E31-9AC8-CBF5795EABBF}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="N5">
-        <v>0.31582600647848219</v>
+        <v>9.3706617306802395E-2</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N6">
-        <v>8.8500694123091153E-2</v>
+        <v>0.40439611291068944</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="N7">
-        <v>0.4043961129106895</v>
+        <v>0.31582600647848219</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="N9">
-        <v>9.3706617306802395E-2</v>
+        <v>8.8500694123091153E-2</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E95B3C-7F1B-4BA0-9485-2434D95E0B12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0268D2D-16E0-4515-B77A-683D0884AF9F}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-05 11:26
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69C5867-29D3-4C43-B833-6F3F3C1AE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A0E0B3-F2D9-4C10-AC67-51F8398371A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S4aH2,S6d1115h07,S6d1115h15,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S4c0909h08,S6d1115h08,S1aH3,S4c0909h14,S6d1115h09,S1aH2,S2aH3,S1b0318h10,S3aH3,S4c0909h16,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1b0318h14,S3aH2,S4c0909h12,S6d1115h11,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18</t>
-  </si>
-  <si>
-    <t>S2aH1,S3aH7,S4c0909h21,S5aH8,S1b0318h04,S4aH8,S4c0909h05,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S6d1115h02,S6d1115h22,S6d1115h23,S6d1115h06,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S6aH8,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S1b0318h21,S1aH6,S4c0909h02,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24</t>
+    <t>S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S4aH2,S6d1115h07,S6d1115h15,S1b0318h14,S3aH2,S4c0909h12,S1aH2,S2aH3,S3aH3,S4c0909h16,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S6d1115h11,S4c0909h08,S6d1115h08,S1aH3,S4c0909h14,S6d1115h09,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h10,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1b0318h13,S3aH5,S4c0909h11,S5aH3</t>
+  </si>
+  <si>
+    <t>S6d1115h06,S2aH1,S3aH7,S4c0909h21,S5aH8,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1b0318h04,S4aH8,S4c0909h05,S1aH6,S4c0909h02,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S6d1115h02,S6d1115h22,S6d1115h23,S6aH8,S1b0318h21,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S2aH1,S3aH7,S4c0909h21,S5aH8,S1b0318h04,S4aH8,S4c0909h05,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S6d1115h02,S6d1115h22,S6d1115h23,S6d1115h06,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S6aH8,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S1b0318h21,S1aH6,S4c0909h02,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24</v>
+        <v>S6d1115h06,S2aH1,S3aH7,S4c0909h21,S5aH8,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1b0318h04,S4aH8,S4c0909h05,S1aH6,S4c0909h02,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S6d1115h02,S6d1115h22,S6d1115h23,S6aH8,S1b0318h21,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S4aH2,S6d1115h07,S6d1115h15,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S4c0909h08,S6d1115h08,S1aH3,S4c0909h14,S6d1115h09,S1aH2,S2aH3,S1b0318h10,S3aH3,S4c0909h16,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1b0318h14,S3aH2,S4c0909h12,S6d1115h11,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18</v>
+        <v>S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S4aH2,S6d1115h07,S6d1115h15,S1b0318h14,S3aH2,S4c0909h12,S1aH2,S2aH3,S3aH3,S4c0909h16,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S6d1115h11,S4c0909h08,S6d1115h08,S1aH3,S4c0909h14,S6d1115h09,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h10,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1b0318h13,S3aH5,S4c0909h11,S5aH3</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E83548-7D24-4153-9F00-316021126006}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02F953-7A56-409D-A11A-E6A0B8082A5B}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912B446D-27B7-4E31-9AC8-CBF5795EABBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4321E20-4B23-49FC-B21F-5346FB6DD1B5}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="N4">
-        <v>0.13490282276723739</v>
+        <v>0.16266774641369736</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="N5">
-        <v>9.3706617306802395E-2</v>
+        <v>8.8500694123091153E-2</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3018,7 +3018,7 @@
         <v>82</v>
       </c>
       <c r="N6">
-        <v>0.40439611291068944</v>
+        <v>0.4043961129106895</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N7">
-        <v>0.31582600647848219</v>
+        <v>0.13490282276723739</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N8">
-        <v>0.16266774641369736</v>
+        <v>9.3706617306802395E-2</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="N9">
-        <v>8.8500694123091153E-2</v>
+        <v>0.31582600647848219</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0268D2D-16E0-4515-B77A-683D0884AF9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A73D0B53-762A-4683-8E6B-5AC7225E2C07}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-07 16:13
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD209A8-6D29-492F-9945-84F9A0F17E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52B782B-01E2-4E15-9742-4C567C7FFB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1b0318h14,S3aH2,S4c0909h12,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1aH3,S4c0909h14,S6d1115h09,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S4c0909h08,S6d1115h08,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S3aH3,S4c0909h16,S4aH2,S6d1115h07,S6d1115h15,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S6d1115h11,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1aH2,S2aH3,S1b0318h10,S1b0318h13,S3aH5,S4c0909h11,S5aH3</t>
-  </si>
-  <si>
-    <t>S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1b0318h21,S1aH6,S4c0909h02,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S6d1115h02,S6d1115h22,S6d1115h23,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S6d1115h06,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S2aH1,S3aH7,S4c0909h21,S5aH8,S1b0318h04,S4aH8,S4c0909h05,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S6aH8,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03</t>
+    <t>S1b0318h14,S3aH2,S4c0909h12,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4c0909h08,S6d1115h08,S4aH2,S6d1115h07,S6d1115h15,S6d1115h11,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1b0318h10,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1aH3,S4c0909h14,S6d1115h09,S3aH3,S4c0909h16,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S1aH2,S2aH3,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2</t>
+  </si>
+  <si>
+    <t>S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S2aH1,S3aH7,S4c0909h21,S5aH8,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S6aH8,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S6d1115h02,S6d1115h22,S6d1115h23,S1b0318h21,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1b0318h04,S4aH8,S4c0909h05,S6d1115h06,S1aH6,S4c0909h02</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1b0318h21,S1aH6,S4c0909h02,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S6d1115h02,S6d1115h22,S6d1115h23,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S6d1115h06,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S2aH1,S3aH7,S4c0909h21,S5aH8,S1b0318h04,S4aH8,S4c0909h05,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S6aH8,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03</v>
+        <v>S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S2aH1,S3aH7,S4c0909h21,S5aH8,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S6aH8,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S6d1115h02,S6d1115h22,S6d1115h23,S1b0318h21,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1b0318h04,S4aH8,S4c0909h05,S6d1115h06,S1aH6,S4c0909h02</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1b0318h14,S3aH2,S4c0909h12,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1aH3,S4c0909h14,S6d1115h09,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S4c0909h08,S6d1115h08,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S3aH3,S4c0909h16,S4aH2,S6d1115h07,S6d1115h15,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S6d1115h11,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1aH2,S2aH3,S1b0318h10,S1b0318h13,S3aH5,S4c0909h11,S5aH3</v>
+        <v>S1b0318h14,S3aH2,S4c0909h12,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4c0909h08,S6d1115h08,S4aH2,S6d1115h07,S6d1115h15,S6d1115h11,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1b0318h10,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1aH3,S4c0909h14,S6d1115h09,S3aH3,S4c0909h16,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S1aH2,S2aH3,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14F91E2-9886-4804-B2BF-C2D5071C175E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E437A9-E70C-4620-972C-3009183C6EC8}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D333AC1-2790-4B7B-806C-CC654EAC7A49}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DCC39B-A105-49EF-8EF5-7333961113E0}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="N4">
-        <v>0.40439611291068944</v>
+        <v>0.16266774641369736</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N5">
-        <v>0.16266774641369736</v>
+        <v>8.8500694123091153E-2</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N6">
-        <v>8.8500694123091153E-2</v>
+        <v>0.40439611291068944</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0EB673-43D0-4398-B958-4A71A7305517}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A0DD91-48D8-4700-A797-F915635A2003}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-10 01:40
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_ITA/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A507D68-9082-4CFA-8EAD-913458FC7385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BE3469-B51B-416E-A0B4-4D40049C7A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -543,21 +543,21 @@
     <t>com_fr</t>
   </si>
   <si>
+    <t>process</t>
+  </si>
+  <si>
     <t>commodity</t>
   </si>
   <si>
-    <t>process</t>
-  </si>
-  <si>
     <t>S1aH1</t>
   </si>
   <si>
+    <t>IMPNRGZ</t>
+  </si>
+  <si>
     <t>elc_sol-ITA</t>
   </si>
   <si>
-    <t>IMPNRGZ</t>
-  </si>
-  <si>
     <t>S1aH2</t>
   </si>
   <si>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH3,S4c0909h14,S6d1115h09,S1aH2,S2aH3,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S3aH3,S4c0909h16,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S4c0909h08,S6d1115h08,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S4aH2,S6d1115h07,S6d1115h15,S1b0318h14,S3aH2,S4c0909h12,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h10,S6d1115h11</t>
-  </si>
-  <si>
-    <t>S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S1b0318h04,S4aH8,S4c0909h05,S1b0318h21,S6d1115h06,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1aH6,S4c0909h02,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S2aH1,S3aH7,S4c0909h21,S5aH8,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S6d1115h02,S6d1115h22,S6d1115h23,S6aH8,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20</t>
+    <t>S1aH2,S2aH3,S3aH3,S4c0909h16,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1aH3,S4c0909h14,S6d1115h09,S4aH2,S6d1115h07,S6d1115h15,S6d1115h11,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4c0909h08,S6d1115h08,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h10,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S1b0318h14,S3aH2,S4c0909h12</t>
+  </si>
+  <si>
+    <t>S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S1aH6,S4c0909h02,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S2aH1,S3aH7,S4c0909h21,S5aH8,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h21,S1b0318h04,S4aH8,S4c0909h05,S6d1115h06,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S6d1115h02,S6d1115h22,S6d1115h23,S6aH8,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S1b0318h04,S4aH8,S4c0909h05,S1b0318h21,S6d1115h06,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1aH6,S4c0909h02,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S2aH1,S3aH7,S4c0909h21,S5aH8,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20,S6d1115h02,S6d1115h22,S6d1115h23,S6aH8,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20</v>
+        <v>S1b0318h06,S4aH6,S6d1115h05,S6d1115h19,S1b0318h01,S2aH8,S4c0909h19,S4c0909h24,S1aH6,S4c0909h02,S1aH7,S3aH6,S4aH7,S4c0909h23,S5aH6,S5aH7,S6aH6,S2aH1,S3aH7,S4c0909h21,S5aH8,S1aH1,S1b0318h03,S1b0318h22,S2aH7,S4c0909h20,S1b0318h21,S1b0318h04,S4aH8,S4c0909h05,S6d1115h06,S1b0318h05,S1b0318h19,S1b0318h20,S4aH1,S4c0909h03,S4c0909h04,S6aH1,S6d1115h21,S6d1115h24,S1b0318h02,S1b0318h23,S2aH6,S3aH1,S4c0909h06,S4c0909h22,S6d1115h02,S6d1115h22,S6d1115h23,S6aH8,S1aH8,S1b0318h24,S5aH1,S6aH7,S6d1115h03,S3aH8,S4c0909h01,S6d1115h01,S6d1115h04,S6d1115h20</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH3,S4c0909h14,S6d1115h09,S1aH2,S2aH3,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S3aH3,S4c0909h16,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S4c0909h08,S6d1115h08,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S4aH2,S6d1115h07,S6d1115h15,S1b0318h14,S3aH2,S4c0909h12,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h10,S6d1115h11</v>
+        <v>S1aH2,S2aH3,S3aH3,S4c0909h16,S1b0318h09,S1b0318h12,S1b0318h16,S6d1115h18,S1aH5,S1b0318h18,S2aH4,S2aH5,S4c0909h10,S5aH2,S5aH5,S6aH2,S1aH3,S4c0909h14,S6d1115h09,S4aH2,S6d1115h07,S6d1115h15,S6d1115h11,S1b0318h08,S5aH4,S6aH3,S6aH4,S6d1115h16,S6d1115h17,S1b0318h17,S4c0909h15,S6aH5,S6d1115h14,S1b0318h07,S3aH4,S4aH3,S4aH4,S4c0909h09,S4c0909h18,S1aH4,S1b0318h11,S1b0318h15,S2aH2,S6d1115h12,S6d1115h13,S4c0909h08,S6d1115h08,S4aH5,S4c0909h07,S4c0909h13,S4c0909h17,S6d1115h10,S1b0318h10,S1b0318h13,S3aH5,S4c0909h11,S5aH3,S1b0318h14,S3aH2,S4c0909h12</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FFF843-3C8F-4B13-B3FD-A5A882A5E522}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04523D2-CAA3-4EC2-8556-66275CB9220F}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B9190B-CDBB-405A-A5AB-B3ACD96BEA33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F913A3-8C27-48A8-B1E7-4DDDD2A52255}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2939,16 +2939,16 @@
         <v>7.9672999999999994E-2</v>
       </c>
       <c r="J4" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K4" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
       <c r="M4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N4">
-        <v>0.40439611291068944</v>
+        <v>0.13490282276723739</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2974,10 +2974,10 @@
         <v>1.0182999999999999E-2</v>
       </c>
       <c r="J5" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K5" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
       <c r="M5" t="s">
         <v>84</v>
@@ -3009,16 +3009,16 @@
         <v>1.4832999999999999E-2</v>
       </c>
       <c r="J6" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K6" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
       <c r="M6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N6">
-        <v>8.8500694123091153E-2</v>
+        <v>0.40439611291068944</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3044,10 +3044,10 @@
         <v>0.20507</v>
       </c>
       <c r="J7" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K7" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
       <c r="M7" t="s">
         <v>87</v>
@@ -3079,16 +3079,16 @@
         <v>2.7425999999999999E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K8" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
       <c r="M8" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="N8">
-        <v>0.13490282276723739</v>
+        <v>8.8500694123091153E-2</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3114,10 +3114,10 @@
         <v>2.299E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K9" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
       <c r="M9" t="s">
         <v>76</v>
@@ -3149,10 +3149,10 @@
         <v>2.2040000000000001E-2</v>
       </c>
       <c r="J10" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K10" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.45">
@@ -3175,10 +3175,10 @@
         <v>6.5097000000000002E-2</v>
       </c>
       <c r="J11" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K11" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.45">
@@ -3201,10 +3201,10 @@
         <v>1.6739999999999999E-3</v>
       </c>
       <c r="J12" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K12" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.45">
@@ -3227,10 +3227,10 @@
         <v>1.8799999999999999E-3</v>
       </c>
       <c r="J13" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K13" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.45">
@@ -3253,10 +3253,10 @@
         <v>2.1549999999999998E-3</v>
       </c>
       <c r="J14" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K14" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.45">
@@ -3279,10 +3279,10 @@
         <v>2.0939999999999999E-3</v>
       </c>
       <c r="J15" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K15" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.45">
@@ -3305,10 +3305,10 @@
         <v>2.4559999999999998E-3</v>
       </c>
       <c r="J16" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K16" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.45">
@@ -3331,10 +3331,10 @@
         <v>2.4559999999999998E-3</v>
       </c>
       <c r="J17" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K17" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.45">
@@ -3357,10 +3357,10 @@
         <v>2.3410000000000002E-3</v>
       </c>
       <c r="J18" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K18" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.45">
@@ -3383,10 +3383,10 @@
         <v>2.4559999999999998E-3</v>
       </c>
       <c r="J19" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K19" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.45">
@@ -3409,10 +3409,10 @@
         <v>2.3939999999999999E-3</v>
       </c>
       <c r="J20" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K20" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.45">
@@ -3435,10 +3435,10 @@
         <v>2.1549999999999998E-3</v>
       </c>
       <c r="J21" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K21" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.45">
@@ -3461,10 +3461,10 @@
         <v>2.0939999999999999E-3</v>
       </c>
       <c r="J22" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K22" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.45">
@@ -3487,10 +3487,10 @@
         <v>2.2790000000000002E-3</v>
       </c>
       <c r="J23" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K23" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.45">
@@ -3513,10 +3513,10 @@
         <v>2.1549999999999998E-3</v>
       </c>
       <c r="J24" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K24" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.45">
@@ -3539,10 +3539,10 @@
         <v>2.3939999999999999E-3</v>
       </c>
       <c r="J25" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K25" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.45">
@@ -3565,10 +3565,10 @@
         <v>1.8339999999999999E-3</v>
       </c>
       <c r="J26" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K26" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.45">
@@ -3591,10 +3591,10 @@
         <v>1.6199999999999999E-3</v>
       </c>
       <c r="J27" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K27" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.45">
@@ -3617,10 +3617,10 @@
         <v>9.3999999999999997E-4</v>
       </c>
       <c r="J28" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K28" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.45">
@@ -3643,10 +3643,10 @@
         <v>5.6800000000000004E-4</v>
       </c>
       <c r="J29" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K29" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.45">
@@ -3669,10 +3669,10 @@
         <v>8.34E-4</v>
       </c>
       <c r="J30" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K30" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.45">
@@ -3695,10 +3695,10 @@
         <v>8.34E-4</v>
       </c>
       <c r="J31" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K31" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.45">
@@ -3721,10 +3721,10 @@
         <v>9.3999999999999997E-4</v>
       </c>
       <c r="J32" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K32" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.45">
@@ -3747,10 +3747,10 @@
         <v>1.121E-3</v>
       </c>
       <c r="J33" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K33" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.45">
@@ -3773,10 +3773,10 @@
         <v>9.3999999999999997E-4</v>
       </c>
       <c r="J34" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K34" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.45">
@@ -3799,10 +3799,10 @@
         <v>6.7100000000000005E-4</v>
       </c>
       <c r="J35" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K35" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.45">
@@ -3825,10 +3825,10 @@
         <v>6.842E-3</v>
       </c>
       <c r="J36" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K36" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.45">
@@ -3851,10 +3851,10 @@
         <v>2.1950000000000003E-3</v>
       </c>
       <c r="J37" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K37" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.45">
@@ -3877,10 +3877,10 @@
         <v>3.64E-3</v>
       </c>
       <c r="J38" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K38" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.45">
@@ -3903,10 +3903,10 @@
         <v>6.4935000000000007E-2</v>
       </c>
       <c r="J39" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K39" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.45">
@@ -3929,10 +3929,10 @@
         <v>1.0637000000000001E-2</v>
       </c>
       <c r="J40" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K40" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.45">
@@ -3955,10 +3955,10 @@
         <v>8.3940000000000004E-3</v>
       </c>
       <c r="J41" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K41" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.45">
@@ -3981,10 +3981,10 @@
         <v>6.3160000000000004E-3</v>
       </c>
       <c r="J42" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K42" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.45">
@@ -4007,10 +4007,10 @@
         <v>8.7559999999999999E-3</v>
       </c>
       <c r="J43" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K43" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.45">
@@ -4033,10 +4033,10 @@
         <v>3.2169999999999998E-3</v>
       </c>
       <c r="J44" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K44" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.45">
@@ -4059,10 +4059,10 @@
         <v>5.2099999999999998E-4</v>
       </c>
       <c r="J45" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K45" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.45">
@@ -4085,10 +4085,10 @@
         <v>6.6699999999999995E-4</v>
       </c>
       <c r="J46" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K46" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.45">
@@ -4111,10 +4111,10 @@
         <v>5.2409999999999998E-2</v>
       </c>
       <c r="J47" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K47" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.45">
@@ -4137,10 +4137,10 @@
         <v>1.4343E-2</v>
       </c>
       <c r="J48" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K48" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.45">
@@ -4163,10 +4163,10 @@
         <v>1.094E-2</v>
       </c>
       <c r="J49" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K49" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.45">
@@ -4189,10 +4189,10 @@
         <v>6.3619999999999996E-3</v>
       </c>
       <c r="J50" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K50" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.45">
@@ -4215,10 +4215,10 @@
         <v>5.2610000000000001E-3</v>
       </c>
       <c r="J51" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K51" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.45">
@@ -4241,10 +4241,10 @@
         <v>1.0709999999999999E-3</v>
       </c>
       <c r="J52" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K52" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.45">
@@ -4267,10 +4267,10 @@
         <v>5.5599999999999996E-4</v>
       </c>
       <c r="J53" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K53" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.45">
@@ -4293,10 +4293,10 @@
         <v>2.5249999999999999E-3</v>
       </c>
       <c r="J54" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K54" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.45">
@@ -4319,10 +4319,10 @@
         <v>3.3578999999999998E-2</v>
       </c>
       <c r="J55" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K55" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.45">
@@ -4345,10 +4345,10 @@
         <v>4.0569999999999998E-3</v>
       </c>
       <c r="J56" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K56" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.45">
@@ -4371,10 +4371,10 @@
         <v>2.382E-3</v>
       </c>
       <c r="J57" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K57" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.45">
@@ -4397,10 +4397,10 @@
         <v>1.1900000000000001E-3</v>
       </c>
       <c r="J58" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K58" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.45">
@@ -4423,10 +4423,10 @@
         <v>1.4010000000000001E-3</v>
       </c>
       <c r="J59" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K59" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.45">
@@ -4449,10 +4449,10 @@
         <v>0</v>
       </c>
       <c r="J60" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K60" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.45">
@@ -4475,10 +4475,10 @@
         <v>0</v>
       </c>
       <c r="J61" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K61" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.45">
@@ -4501,10 +4501,10 @@
         <v>0</v>
       </c>
       <c r="J62" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K62" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.45">
@@ -4527,10 +4527,10 @@
         <v>0</v>
       </c>
       <c r="J63" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K63" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.45">
@@ -4553,10 +4553,10 @@
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="J64" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K64" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.45">
@@ -4579,10 +4579,10 @@
         <v>0</v>
       </c>
       <c r="J65" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K65" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.45">
@@ -4605,10 +4605,10 @@
         <v>0</v>
       </c>
       <c r="J66" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K66" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.45">
@@ -4631,10 +4631,10 @@
         <v>0</v>
       </c>
       <c r="J67" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K67" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.45">
@@ -4657,10 +4657,10 @@
         <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K68" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.45">
@@ -4683,10 +4683,10 @@
         <v>4.1999999999999998E-5</v>
       </c>
       <c r="J69" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K69" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.45">
@@ -4709,10 +4709,10 @@
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="J70" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K70" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.45">
@@ -4735,10 +4735,10 @@
         <v>3.0200000000000002E-4</v>
       </c>
       <c r="J71" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K71" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.45">
@@ -4761,10 +4761,10 @@
         <v>4.3399999999999998E-4</v>
       </c>
       <c r="J72" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K72" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.45">
@@ -4787,10 +4787,10 @@
         <v>5.9500000000000004E-4</v>
       </c>
       <c r="J73" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K73" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.45">
@@ -4813,10 +4813,10 @@
         <v>6.4800000000000003E-4</v>
       </c>
       <c r="J74" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K74" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.45">
@@ -4839,10 +4839,10 @@
         <v>4.3399999999999998E-4</v>
       </c>
       <c r="J75" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K75" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.45">
@@ -4865,10 +4865,10 @@
         <v>4.6099999999999998E-4</v>
       </c>
       <c r="J76" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K76" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.45">
@@ -4891,10 +4891,10 @@
         <v>2.8299999999999999E-4</v>
       </c>
       <c r="J77" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K77" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.45">
@@ -4917,10 +4917,10 @@
         <v>2.1699999999999999E-4</v>
       </c>
       <c r="J78" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K78" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.45">
@@ -4943,10 +4943,10 @@
         <v>8.7000000000000001E-5</v>
       </c>
       <c r="J79" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K79" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.45">
@@ -4969,10 +4969,10 @@
         <v>1.9000000000000001E-5</v>
       </c>
       <c r="J80" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K80" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.45">
@@ -4995,10 +4995,10 @@
         <v>3.4E-5</v>
       </c>
       <c r="J81" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K81" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.45">
@@ -5021,10 +5021,10 @@
         <v>2.8E-5</v>
       </c>
       <c r="J82" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K82" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.45">
@@ -5047,10 +5047,10 @@
         <v>2.0999999999999999E-5</v>
       </c>
       <c r="J83" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K83" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.45">
@@ -5073,10 +5073,10 @@
         <v>4.5700000000000003E-3</v>
       </c>
       <c r="J84" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K84" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.45">
@@ -5099,10 +5099,10 @@
         <v>8.3200000000000006E-4</v>
       </c>
       <c r="J85" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K85" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.45">
@@ -5125,10 +5125,10 @@
         <v>1.1949999999999999E-3</v>
       </c>
       <c r="J86" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K86" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.45">
@@ -5151,10 +5151,10 @@
         <v>1.5807000000000002E-2</v>
       </c>
       <c r="J87" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K87" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.45">
@@ -5177,10 +5177,10 @@
         <v>1.531E-3</v>
       </c>
       <c r="J88" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K88" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.45">
@@ -5203,10 +5203,10 @@
         <v>9.4699999999999993E-4</v>
       </c>
       <c r="J89" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K89" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.45">
@@ -5229,10 +5229,10 @@
         <v>6.8599999999999998E-4</v>
       </c>
       <c r="J90" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K90" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.45">
@@ -5255,10 +5255,10 @@
         <v>2.5869999999999999E-3</v>
       </c>
       <c r="J91" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K91" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.45">
@@ -5281,10 +5281,10 @@
         <v>6.3690999999999998E-2</v>
       </c>
       <c r="J92" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K92" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.45">
@@ -5307,10 +5307,10 @@
         <v>6.6660000000000001E-3</v>
       </c>
       <c r="J93" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K93" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.45">
@@ -5333,10 +5333,10 @@
         <v>5.6349999999999994E-3</v>
       </c>
       <c r="J94" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K94" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.45">
@@ -5359,10 +5359,10 @@
         <v>7.4008000000000004E-2</v>
       </c>
       <c r="J95" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K95" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.45">
@@ -5385,10 +5385,10 @@
         <v>1.0300999999999999E-2</v>
       </c>
       <c r="J96" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K96" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.45">
@@ -5411,10 +5411,10 @@
         <v>1.0467000000000001E-2</v>
       </c>
       <c r="J97" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K97" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.45">
@@ -5437,10 +5437,10 @@
         <v>1.0796E-2</v>
       </c>
       <c r="J98" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K98" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.45">
@@ -5463,10 +5463,10 @@
         <v>4.3207999999999996E-2</v>
       </c>
       <c r="J99" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K99" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.45">
@@ -5489,10 +5489,10 @@
         <v>0</v>
       </c>
       <c r="J100" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K100" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.45">
@@ -5515,10 +5515,10 @@
         <v>0</v>
       </c>
       <c r="J101" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K101" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.45">
@@ -5541,10 +5541,10 @@
         <v>0</v>
       </c>
       <c r="J102" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K102" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.45">
@@ -5567,10 +5567,10 @@
         <v>0</v>
       </c>
       <c r="J103" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K103" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.45">
@@ -5593,10 +5593,10 @@
         <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K104" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.45">
@@ -5619,10 +5619,10 @@
         <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K105" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.45">
@@ -5645,10 +5645,10 @@
         <v>0</v>
       </c>
       <c r="J106" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K106" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.45">
@@ -5671,10 +5671,10 @@
         <v>0</v>
       </c>
       <c r="J107" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K107" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.45">
@@ -5697,10 +5697,10 @@
         <v>0</v>
       </c>
       <c r="J108" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K108" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.45">
@@ -5723,10 +5723,10 @@
         <v>0</v>
       </c>
       <c r="J109" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K109" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="110" spans="2:11" x14ac:dyDescent="0.45">
@@ -5749,10 +5749,10 @@
         <v>0</v>
       </c>
       <c r="J110" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K110" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.45">
@@ -5775,10 +5775,10 @@
         <v>0</v>
       </c>
       <c r="J111" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K111" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.45">
@@ -5801,10 +5801,10 @@
         <v>0</v>
       </c>
       <c r="J112" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K112" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="113" spans="2:11" x14ac:dyDescent="0.45">
@@ -5827,10 +5827,10 @@
         <v>0</v>
       </c>
       <c r="J113" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K113" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="114" spans="2:11" x14ac:dyDescent="0.45">
@@ -5853,10 +5853,10 @@
         <v>0</v>
       </c>
       <c r="J114" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K114" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.45">
@@ -5879,10 +5879,10 @@
         <v>0</v>
       </c>
       <c r="J115" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K115" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.45">
@@ -5905,10 +5905,10 @@
         <v>0</v>
       </c>
       <c r="J116" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K116" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.45">
@@ -5931,10 +5931,10 @@
         <v>0</v>
       </c>
       <c r="J117" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K117" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.45">
@@ -5957,10 +5957,10 @@
         <v>0</v>
       </c>
       <c r="J118" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K118" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.45">
@@ -5983,10 +5983,10 @@
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="J119" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K119" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.45">
@@ -6009,10 +6009,10 @@
         <v>2.0999999999999999E-5</v>
       </c>
       <c r="J120" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K120" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="121" spans="2:11" x14ac:dyDescent="0.45">
@@ -6035,10 +6035,10 @@
         <v>2.8E-5</v>
       </c>
       <c r="J121" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K121" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="122" spans="2:11" x14ac:dyDescent="0.45">
@@ -6061,10 +6061,10 @@
         <v>4.8999999999999998E-5</v>
       </c>
       <c r="J122" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K122" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
     <row r="123" spans="2:11" x14ac:dyDescent="0.45">
@@ -6087,10 +6087,10 @@
         <v>4.1999999999999998E-5</v>
       </c>
       <c r="J123" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="K123" t="s">
-        <v>171</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1620D799-D8E8-4EA2-B5F4-28629CA1F3D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341FEF7E-6ADF-4E05-A1E6-66FA93A50810}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -6128,10 +6128,10 @@
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I3" t="s">
         <v>70</v>
@@ -6140,7 +6140,7 @@
         <v>166</v>
       </c>
       <c r="M3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N3" t="s">
         <v>70</v>

</xml_diff>